<commit_message>
Removed unncessary duplicates of YNM_Sales_Final and YNE_Sales_Final csv files. Changed file path in main to get the final sales from the SheetPreprocessor
</commit_message>
<xml_diff>
--- a/YNM_Payout_Prototype.xlsx
+++ b/YNM_Payout_Prototype.xlsx
@@ -2319,19 +2319,19 @@
         <v>-0.16</v>
       </c>
       <c r="F57" t="n">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="G57" t="n">
-        <v>-6.68</v>
+        <v>-5.18</v>
       </c>
       <c r="H57" s="3" t="n">
-        <v>-2.672</v>
+        <v>-2.072</v>
       </c>
       <c r="I57" t="n">
-        <v>-3.34</v>
+        <v>-2.59</v>
       </c>
       <c r="J57" t="n">
-        <v>-4.008</v>
+        <v>-3.108</v>
       </c>
     </row>
     <row r="58">
@@ -2379,7 +2379,7 @@
         </is>
       </c>
       <c r="J59" s="4" t="n">
-        <v>12.764</v>
+        <v>13.364</v>
       </c>
     </row>
     <row r="60">
@@ -4528,19 +4528,19 @@
         <v>-0.16</v>
       </c>
       <c r="F26" t="n">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="G26" t="n">
-        <v>-6.68</v>
+        <v>-5.18</v>
       </c>
       <c r="H26" s="3" t="n">
-        <v>-2.672</v>
+        <v>-2.072</v>
       </c>
       <c r="I26" t="n">
-        <v>-3.34</v>
+        <v>-2.59</v>
       </c>
       <c r="J26" t="n">
-        <v>-4.008</v>
+        <v>-3.108</v>
       </c>
     </row>
     <row r="27">
@@ -4550,7 +4550,7 @@
         </is>
       </c>
       <c r="J27" s="4" t="n">
-        <v>-11.344</v>
+        <v>-10.744</v>
       </c>
     </row>
     <row r="28">
@@ -8771,19 +8771,19 @@
         <v>0.46</v>
       </c>
       <c r="F40" t="n">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="G40" t="n">
-        <v>12.47</v>
+        <v>14.97</v>
       </c>
       <c r="H40" t="n">
-        <v>4.988</v>
+        <v>5.988</v>
       </c>
       <c r="I40" t="n">
-        <v>6.234999999999999</v>
+        <v>7.484999999999999</v>
       </c>
       <c r="J40" s="3" t="n">
-        <v>7.481999999999999</v>
+        <v>8.981999999999999</v>
       </c>
     </row>
     <row r="41">
@@ -8809,19 +8809,19 @@
         <v>2.73</v>
       </c>
       <c r="F41" t="n">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="G41" t="n">
-        <v>73.41</v>
+        <v>88.41</v>
       </c>
       <c r="H41" t="n">
-        <v>29.364</v>
+        <v>35.364</v>
       </c>
       <c r="I41" t="n">
-        <v>36.705</v>
+        <v>44.205</v>
       </c>
       <c r="J41" s="3" t="n">
-        <v>44.046</v>
+        <v>53.046</v>
       </c>
     </row>
     <row r="42">
@@ -9249,7 +9249,7 @@
         </is>
       </c>
       <c r="J53" s="4" t="n">
-        <v>320.076</v>
+        <v>330.576</v>
       </c>
     </row>
     <row r="54">
@@ -13935,19 +13935,19 @@
         <v>9.83</v>
       </c>
       <c r="F198" t="n">
-        <v>130</v>
+        <v>0</v>
       </c>
       <c r="G198" t="n">
-        <v>187.77</v>
+        <v>317.77</v>
       </c>
       <c r="H198" t="n">
-        <v>75.10800000000002</v>
+        <v>127.108</v>
       </c>
       <c r="I198" t="n">
-        <v>93.88500000000002</v>
+        <v>158.885</v>
       </c>
       <c r="J198" s="3" t="n">
-        <v>112.662</v>
+        <v>190.662</v>
       </c>
     </row>
     <row r="199">
@@ -13973,19 +13973,19 @@
         <v>6.75</v>
       </c>
       <c r="F199" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="G199" t="n">
-        <v>128.25</v>
+        <v>218.25</v>
       </c>
       <c r="H199" t="n">
-        <v>51.3</v>
+        <v>87.30000000000001</v>
       </c>
       <c r="I199" t="n">
-        <v>64.125</v>
+        <v>109.125</v>
       </c>
       <c r="J199" s="3" t="n">
-        <v>76.95</v>
+        <v>130.95</v>
       </c>
     </row>
     <row r="200">
@@ -13995,7 +13995,7 @@
         </is>
       </c>
       <c r="J200" s="4" t="n">
-        <v>189.612</v>
+        <v>321.612</v>
       </c>
     </row>
     <row r="201">
@@ -16601,19 +16601,19 @@
         <v>0.75</v>
       </c>
       <c r="F285" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G285" t="n">
-        <v>14.25</v>
+        <v>24.25</v>
       </c>
       <c r="H285" t="n">
-        <v>5.7</v>
+        <v>9.700000000000001</v>
       </c>
       <c r="I285" t="n">
-        <v>7.125</v>
+        <v>12.125</v>
       </c>
       <c r="J285" s="3" t="n">
-        <v>8.549999999999999</v>
+        <v>14.55</v>
       </c>
     </row>
     <row r="286">
@@ -16623,7 +16623,7 @@
         </is>
       </c>
       <c r="J286" s="4" t="n">
-        <v>8.549999999999999</v>
+        <v>14.55</v>
       </c>
     </row>
     <row r="287">
@@ -17277,19 +17277,19 @@
         <v>0.45</v>
       </c>
       <c r="F307" t="n">
-        <v>2.5</v>
+        <v>0</v>
       </c>
       <c r="G307" t="n">
-        <v>12.05</v>
+        <v>14.55</v>
       </c>
       <c r="H307" t="n">
-        <v>4.82</v>
+        <v>5.82</v>
       </c>
       <c r="I307" t="n">
-        <v>6.025</v>
+        <v>7.275</v>
       </c>
       <c r="J307" s="3" t="n">
-        <v>7.23</v>
+        <v>8.73</v>
       </c>
     </row>
     <row r="308">
@@ -17413,7 +17413,7 @@
         </is>
       </c>
       <c r="J311" s="4" t="n">
-        <v>67.374</v>
+        <v>68.874</v>
       </c>
     </row>
     <row r="312">
@@ -18597,19 +18597,19 @@
         <v>3.06</v>
       </c>
       <c r="F347" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G347" t="n">
-        <v>58.92999999999999</v>
+        <v>98.92999999999999</v>
       </c>
       <c r="H347" t="n">
-        <v>23.572</v>
+        <v>39.572</v>
       </c>
       <c r="I347" t="n">
-        <v>29.465</v>
+        <v>49.465</v>
       </c>
       <c r="J347" s="3" t="n">
-        <v>35.358</v>
+        <v>59.35799999999999</v>
       </c>
     </row>
     <row r="348">
@@ -18619,7 +18619,7 @@
         </is>
       </c>
       <c r="J348" s="4" t="n">
-        <v>43.90799999999999</v>
+        <v>67.90799999999999</v>
       </c>
     </row>
     <row r="349">
@@ -18709,19 +18709,19 @@
         <v>0.75</v>
       </c>
       <c r="F351" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="G351" t="n">
-        <v>14.25</v>
+        <v>24.25</v>
       </c>
       <c r="H351" t="n">
-        <v>5.7</v>
+        <v>9.700000000000001</v>
       </c>
       <c r="I351" t="n">
-        <v>7.125</v>
+        <v>12.125</v>
       </c>
       <c r="J351" s="3" t="n">
-        <v>8.549999999999999</v>
+        <v>14.55</v>
       </c>
     </row>
     <row r="352">
@@ -18959,7 +18959,7 @@
         </is>
       </c>
       <c r="J358" s="4" t="n">
-        <v>157.98</v>
+        <v>163.98</v>
       </c>
     </row>
     <row r="359">
@@ -19427,19 +19427,19 @@
         <v>3.6</v>
       </c>
       <c r="F372" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="G372" t="n">
-        <v>76.40000000000001</v>
+        <v>116.4</v>
       </c>
       <c r="H372" t="n">
-        <v>30.56</v>
+        <v>46.56</v>
       </c>
       <c r="I372" t="n">
-        <v>38.2</v>
+        <v>58.2</v>
       </c>
       <c r="J372" s="3" t="n">
-        <v>45.84</v>
+        <v>69.84</v>
       </c>
     </row>
     <row r="373">
@@ -19487,7 +19487,7 @@
         </is>
       </c>
       <c r="J374" s="4" t="n">
-        <v>73.83</v>
+        <v>97.83</v>
       </c>
     </row>
     <row r="375">
@@ -19615,19 +19615,19 @@
         <v>0.45</v>
       </c>
       <c r="F378" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G378" t="n">
-        <v>11.55</v>
+        <v>14.55</v>
       </c>
       <c r="H378" t="n">
-        <v>4.62</v>
+        <v>5.82</v>
       </c>
       <c r="I378" t="n">
-        <v>5.775</v>
+        <v>7.275</v>
       </c>
       <c r="J378" s="3" t="n">
-        <v>6.930000000000001</v>
+        <v>8.73</v>
       </c>
     </row>
     <row r="379">
@@ -19637,7 +19637,7 @@
         </is>
       </c>
       <c r="J379" s="4" t="n">
-        <v>20.79</v>
+        <v>22.59</v>
       </c>
     </row>
     <row r="380">
@@ -21343,7 +21343,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>-6.54</v>
+        <v>-5.94</v>
       </c>
     </row>
     <row r="21">
@@ -21493,7 +21493,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>12.76</v>
+        <v>13.36</v>
       </c>
     </row>
     <row r="36">
@@ -21803,7 +21803,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>320.08</v>
+        <v>330.58</v>
       </c>
     </row>
     <row r="67">
@@ -21993,7 +21993,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>189.61</v>
+        <v>321.61</v>
       </c>
     </row>
     <row r="86">
@@ -22163,7 +22163,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>8.550000000000001</v>
+        <v>14.55</v>
       </c>
     </row>
     <row r="103">
@@ -22183,7 +22183,7 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>67.37</v>
+        <v>68.87</v>
       </c>
     </row>
     <row r="105">
@@ -22233,7 +22233,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>43.91</v>
+        <v>67.91</v>
       </c>
     </row>
     <row r="110">
@@ -22243,7 +22243,7 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>157.98</v>
+        <v>163.98</v>
       </c>
     </row>
     <row r="111">
@@ -22253,7 +22253,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>73.83</v>
+        <v>97.83</v>
       </c>
     </row>
     <row r="112">
@@ -22263,7 +22263,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>20.79</v>
+        <v>22.59</v>
       </c>
     </row>
     <row r="113">
@@ -22430,7 +22430,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>-6.544000000000001</v>
+        <v>-5.944</v>
       </c>
     </row>
     <row r="9">

</xml_diff>